<commit_message>
Managing Assets Using Orchestrator API
</commit_message>
<xml_diff>
--- a/Test.xlsx
+++ b/Test.xlsx
@@ -6,7 +6,8 @@
     <x:workbookView firstSheet="0" activeTab="0"/>
   </x:bookViews>
   <x:sheets>
-    <x:sheet name="Folders" sheetId="2" r:id="rId2"/>
+    <x:sheet name="SpecificFolderAsset" sheetId="2" r:id="rId2"/>
+    <x:sheet name="AllFolderAsset" sheetId="5" r:id="rId5"/>
   </x:sheets>
   <x:definedNames/>
   <x:calcPr calcId="125725"/>
@@ -14,18 +15,24 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
-  <x:si>
-    <x:t>Shared</x:t>
-  </x:si>
-  <x:si>
-    <x:t>4765339</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Test</x:t>
-  </x:si>
-  <x:si>
-    <x:t>5002486</x:t>
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+  <x:si>
+    <x:t>TestAddAsset</x:t>
+  </x:si>
+  <x:si>
+    <x:t>902087</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Name</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Id</x:t>
+  </x:si>
+  <x:si>
+    <x:t>TestAddAssetCred</x:t>
+  </x:si>
+  <x:si>
+    <x:t>907838</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -376,7 +383,7 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:B2"/>
+  <x:dimension ref="A1:A1"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
@@ -390,12 +397,48 @@
         <x:v>1</x:v>
       </x:c>
     </x:row>
+  </x:sheetData>
+  <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
+  <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
+  <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>
+  <x:headerFooter/>
+  <x:tableParts count="0"/>
+</x:worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <x:sheetPr>
+    <x:outlinePr summaryBelow="1" summaryRight="1"/>
+  </x:sheetPr>
+  <x:dimension ref="A1:B3"/>
+  <x:sheetViews>
+    <x:sheetView workbookViewId="0"/>
+  </x:sheetViews>
+  <x:sheetFormatPr defaultRowHeight="15"/>
+  <x:sheetData>
+    <x:row r="1" spans="1:2">
+      <x:c r="A1" s="0" t="s">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="B1" s="0" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
     <x:row r="2" spans="1:2">
       <x:c r="A2" s="0" t="s">
-        <x:v>2</x:v>
+        <x:v>0</x:v>
       </x:c>
       <x:c r="B2" s="0" t="s">
-        <x:v>3</x:v>
+        <x:v>1</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="3" spans="1:2">
+      <x:c r="A3" s="0" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="B3" s="0" t="s">
+        <x:v>5</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>